<commit_message>
Removed some print statement
</commit_message>
<xml_diff>
--- a/Tags&Requirements.xlsx
+++ b/Tags&Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\CS481\TARGEST.Final-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{340F9DAC-4997-4AA7-8139-4FC5C348CC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC9E098C-19CC-4B08-A3B0-48065359E491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="735" windowWidth="19185" windowHeight="10065" xr2:uid="{639D7AC7-88DD-43C4-A7F6-5BC14C285E7D}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="19185" windowHeight="10065" xr2:uid="{9001BC15-036B-4D12-80FE-E0745E0BA2D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -1495,7 +1495,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4CA070-97EF-4E10-AF32-AAB6616A9788}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CF777F-13D3-4A00-9A95-D080765F179F}">
   <dimension ref="A1:N122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Added trees in Gui
</commit_message>
<xml_diff>
--- a/Tags&Requirements.xlsx
+++ b/Tags&Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\CS481\TARGEST.Final-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC9E098C-19CC-4B08-A3B0-48065359E491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE125B18-DB90-48E2-B9B7-F25686FC7923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="735" windowWidth="19185" windowHeight="10065" xr2:uid="{9001BC15-036B-4D12-80FE-E0745E0BA2D7}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="19185" windowHeight="10065" xr2:uid="{45C546F5-2AF8-46F0-82C1-28237ED30C21}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -1495,7 +1495,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CF777F-13D3-4A00-9A95-D080765F179F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FC1679-AA68-4C60-A84E-3166AF2C9B9D}">
   <dimension ref="A1:N122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
modified scroolbar textbox in gui
</commit_message>
<xml_diff>
--- a/Tags&Requirements.xlsx
+++ b/Tags&Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\CS481\TARGEST.Final-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE125B18-DB90-48E2-B9B7-F25686FC7923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC37A497-A7E8-4B8F-8639-6A2C9B8B6951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="735" windowWidth="19185" windowHeight="10065" xr2:uid="{45C546F5-2AF8-46F0-82C1-28237ED30C21}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="19185" windowHeight="10065" xr2:uid="{87E44EA6-AFDC-4E7F-B3DB-E5ED6DD1A395}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -1495,7 +1495,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FC1679-AA68-4C60-A84E-3166AF2C9B9D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8E6E00-A690-4E87-BE5D-9D5F351B4168}">
   <dimension ref="A1:N122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Commented out the error line from Tom
</commit_message>
<xml_diff>
--- a/Tags&Requirements.xlsx
+++ b/Tags&Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\CS481\TARGEST.Final-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC37A497-A7E8-4B8F-8639-6A2C9B8B6951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8C37C38-449E-438D-971A-FC3B392FB5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="735" windowWidth="19185" windowHeight="10065" xr2:uid="{87E44EA6-AFDC-4E7F-B3DB-E5ED6DD1A395}"/>
+    <workbookView xWindow="1073" yWindow="1073" windowWidth="14400" windowHeight="7282" xr2:uid="{57E768BD-9CF4-431F-8D6D-6DE6BBAF99BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -1495,7 +1495,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8E6E00-A690-4E87-BE5D-9D5F351B4168}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEDEC20B-46A2-42F9-A8C4-C3528D42E9DF}">
   <dimension ref="A1:N122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Generate report button get disabled after clicked
</commit_message>
<xml_diff>
--- a/Tags&Requirements.xlsx
+++ b/Tags&Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\CS481\TARGEST.Final-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8C37C38-449E-438D-971A-FC3B392FB5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C582F814-0D09-4D9F-86F4-17537CD148EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1073" yWindow="1073" windowWidth="14400" windowHeight="7282" xr2:uid="{57E768BD-9CF4-431F-8D6D-6DE6BBAF99BB}"/>
+    <workbookView xWindow="1073" yWindow="1073" windowWidth="14400" windowHeight="7282" xr2:uid="{26A90D40-2006-4370-A1A8-3138141BFC05}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -1495,7 +1495,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEDEC20B-46A2-42F9-A8C4-C3528D42E9DF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E106F073-C6B1-4BDB-98F0-ACFA463076A6}">
   <dimension ref="A1:N122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>